<commit_message>
added user profile changes (backend) extracted several methods (backend)
</commit_message>
<xml_diff>
--- a/docs/Overwiew_endpoints.xlsx
+++ b/docs/Overwiew_endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\ese2019-team8\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{B5DC8251-7362-486E-BBB3-F9F8283E12C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4130CC71-097A-48CE-BF5B-38744041B4CD}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{B5DC8251-7362-486E-BBB3-F9F8283E12C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{51BE14BD-4E05-440E-AE5C-08E297B5F5A4}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="42">
   <si>
     <t>username</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>token</t>
+  </si>
+  <si>
+    <t>gelb = optional</t>
   </si>
 </sst>
 </file>
@@ -513,9 +516,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B759F60C-B498-4DED-A37F-801BD6AC74F2}">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -673,12 +678,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>3</v>
       </c>
@@ -695,7 +700,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
       <c r="E20">
         <v>200</v>
       </c>
@@ -703,42 +708,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>21</v>
       </c>
@@ -754,12 +759,9 @@
       <c r="F29" t="s">
         <v>7</v>
       </c>
-      <c r="I29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D30" t="s">
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D30" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E30">
@@ -768,201 +770,187 @@
       <c r="F30" t="s">
         <v>38</v>
       </c>
-      <c r="I30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D31" t="s">
+      <c r="H30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D31" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E31">
+        <v>200</v>
+      </c>
+      <c r="G31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="G37" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39">
+        <v>404</v>
+      </c>
+      <c r="F39" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" t="s">
+        <v>25</v>
+      </c>
+      <c r="I39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D40" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40">
         <v>204</v>
       </c>
-      <c r="I31" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D32" t="s">
-        <v>14</v>
-      </c>
-      <c r="I32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D33" t="s">
-        <v>15</v>
-      </c>
-      <c r="I33" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I34" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D35" t="s">
-        <v>17</v>
-      </c>
-      <c r="I35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D36" t="s">
-        <v>18</v>
-      </c>
-      <c r="I36" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="I37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B38" t="s">
-        <v>21</v>
-      </c>
-      <c r="C38" t="s">
-        <v>23</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="F40" t="s">
+        <v>27</v>
+      </c>
+      <c r="I40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" t="s">
         <v>40</v>
       </c>
-      <c r="E38">
+      <c r="E42">
         <v>404</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F42" t="s">
         <v>7</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H42" t="s">
         <v>25</v>
       </c>
-      <c r="I38" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D39" t="s">
-        <v>20</v>
-      </c>
-      <c r="E39">
+      <c r="I42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D43" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43">
         <v>204</v>
       </c>
-      <c r="F39" t="s">
-        <v>27</v>
-      </c>
-      <c r="I39" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="I40" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B41" t="s">
-        <v>24</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="F43" t="s">
+        <v>26</v>
+      </c>
+      <c r="I43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
         <v>12</v>
       </c>
-      <c r="D41" t="s">
+      <c r="G45" t="s">
+        <v>30</v>
+      </c>
+      <c r="I45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I46" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" t="s">
         <v>40</v>
       </c>
-      <c r="E41">
-        <v>404</v>
-      </c>
-      <c r="F41" t="s">
-        <v>7</v>
-      </c>
-      <c r="H41" t="s">
-        <v>25</v>
-      </c>
-      <c r="I41" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>204</v>
-      </c>
-      <c r="F42" t="s">
-        <v>26</v>
-      </c>
-      <c r="I42" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="I43" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" t="s">
-        <v>30</v>
-      </c>
-      <c r="I44" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="I45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B46" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46" t="s">
-        <v>40</v>
-      </c>
-      <c r="E46" s="2">
+      <c r="E47" s="2">
         <v>403</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="I46" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="D47" t="s">
-        <v>0</v>
-      </c>
-      <c r="E47">
-        <v>201</v>
-      </c>
-      <c r="G47" t="s">
-        <v>0</v>
       </c>
       <c r="I47" t="s">
         <v>28</v>
@@ -970,10 +958,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="D48" t="s">
-        <v>34</v>
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>201</v>
       </c>
       <c r="G48" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="I48" t="s">
         <v>28</v>
@@ -981,10 +972,10 @@
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D49" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G49" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I49" t="s">
         <v>28</v>
@@ -992,10 +983,10 @@
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I50" t="s">
         <v>28</v>
@@ -1003,10 +994,10 @@
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I51" t="s">
         <v>28</v>
@@ -1014,49 +1005,46 @@
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D52" t="s">
+        <v>33</v>
+      </c>
+      <c r="G52" t="s">
+        <v>33</v>
+      </c>
+      <c r="I52" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D53" t="s">
         <v>35</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G53" t="s">
         <v>35</v>
       </c>
-      <c r="I52" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.45">
       <c r="I53" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B54" t="s">
+      <c r="I54" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B55" t="s">
         <v>21</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>12</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>40</v>
       </c>
-      <c r="E54" s="2">
+      <c r="E55" s="2">
         <v>404</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F55" t="s">
         <v>36</v>
-      </c>
-      <c r="I54" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D55" t="s">
-        <v>0</v>
-      </c>
-      <c r="E55">
-        <v>403</v>
-      </c>
-      <c r="F55" t="s">
-        <v>38</v>
       </c>
       <c r="I55" t="s">
         <v>28</v>
@@ -1064,10 +1052,13 @@
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D56" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="E56">
-        <v>204</v>
+        <v>403</v>
+      </c>
+      <c r="F56" t="s">
+        <v>38</v>
       </c>
       <c r="I56" t="s">
         <v>28</v>
@@ -1075,7 +1066,10 @@
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D57" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="E57">
+        <v>204</v>
       </c>
       <c r="I57" t="s">
         <v>28</v>
@@ -1083,7 +1077,7 @@
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D58" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I58" t="s">
         <v>28</v>
@@ -1091,7 +1085,7 @@
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D59" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I59" t="s">
         <v>28</v>
@@ -1099,43 +1093,37 @@
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D60" t="s">
+        <v>33</v>
+      </c>
+      <c r="I60" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D61" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="I61" t="s">
-        <v>28</v>
-      </c>
-    </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B62" t="s">
+      <c r="I62" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B63" t="s">
         <v>24</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>12</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D63" t="s">
         <v>40</v>
       </c>
-      <c r="E62">
+      <c r="E63">
         <v>404</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F63" t="s">
         <v>36</v>
-      </c>
-      <c r="I62" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D63" t="s">
-        <v>0</v>
-      </c>
-      <c r="E63">
-        <v>403</v>
-      </c>
-      <c r="F63" t="s">
-        <v>38</v>
       </c>
       <c r="I63" t="s">
         <v>28</v>
@@ -1143,12 +1131,26 @@
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D64" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>403</v>
+      </c>
+      <c r="F64" t="s">
+        <v>38</v>
+      </c>
+      <c r="I64" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="65" spans="4:6" x14ac:dyDescent="0.45">
+      <c r="D65" t="s">
         <v>34</v>
       </c>
-      <c r="E64">
+      <c r="E65">
         <v>204</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F65" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added service model (backend) added service controller (backend)
</commit_message>
<xml_diff>
--- a/docs/Overwiew_endpoints.xlsx
+++ b/docs/Overwiew_endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\ese2019-team8\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{B5DC8251-7362-486E-BBB3-F9F8283E12C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{51BE14BD-4E05-440E-AE5C-08E297B5F5A4}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{B5DC8251-7362-486E-BBB3-F9F8283E12C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1A033702-0FC5-46D9-8B9C-891D9F125D39}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="42">
   <si>
     <t>username</t>
   </si>
@@ -518,9 +518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B759F60C-B498-4DED-A37F-801BD6AC74F2}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD40"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -927,14 +925,6 @@
       <c r="G45" t="s">
         <v>30</v>
       </c>
-      <c r="I45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="I46" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B47" t="s">
@@ -952,9 +942,6 @@
       <c r="F47" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I47" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="D48" t="s">
@@ -966,9 +953,6 @@
       <c r="G48" t="s">
         <v>0</v>
       </c>
-      <c r="I48" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D49" t="s">
@@ -977,9 +961,6 @@
       <c r="G49" t="s">
         <v>34</v>
       </c>
-      <c r="I49" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D50" t="s">
@@ -988,9 +969,6 @@
       <c r="G50" t="s">
         <v>31</v>
       </c>
-      <c r="I50" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D51" t="s">
@@ -999,9 +977,6 @@
       <c r="G51" t="s">
         <v>32</v>
       </c>
-      <c r="I51" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D52" t="s">
@@ -1010,9 +985,6 @@
       <c r="G52" t="s">
         <v>33</v>
       </c>
-      <c r="I52" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D53" t="s">
@@ -1020,14 +992,6 @@
       </c>
       <c r="G53" t="s">
         <v>35</v>
-      </c>
-      <c r="I53" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="I54" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
added PUT service (backend)
</commit_message>
<xml_diff>
--- a/docs/Overwiew_endpoints.xlsx
+++ b/docs/Overwiew_endpoints.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\ese2019-team8\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a5b6fa8fcd6b6a78/Dokumente/GitHub/ese2019-team8/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{B5DC8251-7362-486E-BBB3-F9F8283E12C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1A033702-0FC5-46D9-8B9C-891D9F125D39}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="13_ncr:1_{B5DC8251-7362-486E-BBB3-F9F8283E12C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{221D0A39-7012-42C9-8EA0-CC8E2DD77FCD}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="44">
   <si>
     <t>username</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>gelb = optional</t>
+  </si>
+  <si>
+    <t>/search</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -516,9 +522,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B759F60C-B498-4DED-A37F-801BD6AC74F2}">
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -936,104 +944,89 @@
       <c r="D47" t="s">
         <v>40</v>
       </c>
-      <c r="E47" s="2">
-        <v>403</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>38</v>
+      <c r="E47">
+        <v>404</v>
+      </c>
+      <c r="F47" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="D48" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E48">
-        <v>201</v>
-      </c>
-      <c r="G48" t="s">
-        <v>0</v>
+        <v>403</v>
+      </c>
+      <c r="F48" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D49" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="E49">
+        <v>201</v>
       </c>
       <c r="G49" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D50" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G50" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D51" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G51" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D52" t="s">
+        <v>35</v>
+      </c>
+      <c r="G52" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="G53" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="G54" t="s">
         <v>33</v>
       </c>
-      <c r="G52" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D53" t="s">
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="G55" t="s">
         <v>35</v>
       </c>
-      <c r="G53" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B55" t="s">
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B57" t="s">
         <v>21</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C57" t="s">
         <v>12</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D57" t="s">
         <v>40</v>
       </c>
-      <c r="E55" s="2">
+      <c r="E57" s="2">
         <v>404</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F57" t="s">
         <v>36</v>
-      </c>
-      <c r="I55" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D56" t="s">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>403</v>
-      </c>
-      <c r="F56" t="s">
-        <v>38</v>
-      </c>
-      <c r="I56" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D57" t="s">
-        <v>34</v>
-      </c>
-      <c r="E57">
-        <v>204</v>
       </c>
       <c r="I57" t="s">
         <v>28</v>
@@ -1041,7 +1034,13 @@
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D58" t="s">
-        <v>31</v>
+        <v>43</v>
+      </c>
+      <c r="E58">
+        <v>404</v>
+      </c>
+      <c r="F58" t="s">
+        <v>7</v>
       </c>
       <c r="I58" t="s">
         <v>28</v>
@@ -1049,7 +1048,13 @@
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D59" t="s">
-        <v>32</v>
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>403</v>
+      </c>
+      <c r="F59" t="s">
+        <v>39</v>
       </c>
       <c r="I59" t="s">
         <v>28</v>
@@ -1057,7 +1062,13 @@
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D60" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="E60">
+        <v>204</v>
+      </c>
+      <c r="G60" t="s">
+        <v>43</v>
       </c>
       <c r="I60" t="s">
         <v>28</v>
@@ -1065,29 +1076,32 @@
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D61" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="G61" t="s">
+        <v>0</v>
+      </c>
+      <c r="I61" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D62" t="s">
+        <v>32</v>
+      </c>
+      <c r="G62" t="s">
+        <v>34</v>
+      </c>
       <c r="I62" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B63" t="s">
-        <v>24</v>
-      </c>
-      <c r="C63" t="s">
-        <v>12</v>
-      </c>
       <c r="D63" t="s">
-        <v>40</v>
-      </c>
-      <c r="E63">
-        <v>404</v>
-      </c>
-      <c r="F63" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="G63" t="s">
+        <v>31</v>
       </c>
       <c r="I63" t="s">
         <v>28</v>
@@ -1095,27 +1109,149 @@
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D64" t="s">
+        <v>35</v>
+      </c>
+      <c r="G64" t="s">
+        <v>32</v>
+      </c>
+      <c r="I64" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="G65" t="s">
+        <v>33</v>
+      </c>
+      <c r="I65" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="G66" t="s">
+        <v>35</v>
+      </c>
+      <c r="I66" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="I67" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B68" t="s">
+        <v>24</v>
+      </c>
+      <c r="C68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" t="s">
+        <v>40</v>
+      </c>
+      <c r="E68">
+        <v>404</v>
+      </c>
+      <c r="F68" t="s">
+        <v>36</v>
+      </c>
+      <c r="I68" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D69" t="s">
         <v>0</v>
       </c>
-      <c r="E64">
+      <c r="E69">
         <v>403</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F69" t="s">
         <v>38</v>
       </c>
-      <c r="I64" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="65" spans="4:6" x14ac:dyDescent="0.45">
-      <c r="D65" t="s">
+      <c r="I69" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D70" t="s">
         <v>34</v>
       </c>
-      <c r="E65">
+      <c r="E70">
         <v>204</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F70" t="s">
         <v>37</v>
+      </c>
+      <c r="I70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="I71" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B72" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" t="s">
+        <v>42</v>
+      </c>
+      <c r="D72" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>200</v>
+      </c>
+      <c r="I72" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D73" t="s">
+        <v>34</v>
+      </c>
+      <c r="I73" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D74" t="s">
+        <v>31</v>
+      </c>
+      <c r="I74" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D75" t="s">
+        <v>32</v>
+      </c>
+      <c r="I75" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D76" t="s">
+        <v>33</v>
+      </c>
+      <c r="I76" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D77" t="s">
+        <v>35</v>
+      </c>
+      <c r="I77" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="I78" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added DELETE service (backend)
</commit_message>
<xml_diff>
--- a/docs/Overwiew_endpoints.xlsx
+++ b/docs/Overwiew_endpoints.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a5b6fa8fcd6b6a78/Dokumente/GitHub/ese2019-team8/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\ese2019-team8\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="13_ncr:1_{B5DC8251-7362-486E-BBB3-F9F8283E12C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{221D0A39-7012-42C9-8EA0-CC8E2DD77FCD}"/>
+  <xr:revisionPtr revIDLastSave="130" documentId="13_ncr:1_{B5DC8251-7362-486E-BBB3-F9F8283E12C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1EFD8973-CDF8-4DE6-A7F4-79074428D0B8}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="44">
   <si>
     <t>username</t>
   </si>
@@ -522,11 +522,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B759F60C-B498-4DED-A37F-801BD6AC74F2}">
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -962,7 +960,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D49" t="s">
         <v>31</v>
       </c>
@@ -973,7 +971,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D50" t="s">
         <v>32</v>
       </c>
@@ -981,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D51" t="s">
         <v>33</v>
       </c>
@@ -989,7 +987,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D52" t="s">
         <v>35</v>
       </c>
@@ -997,22 +995,22 @@
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G53" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G54" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G55" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B57" t="s">
         <v>21</v>
       </c>
@@ -1028,11 +1026,8 @@
       <c r="F57" t="s">
         <v>36</v>
       </c>
-      <c r="I57" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D58" t="s">
         <v>43</v>
       </c>
@@ -1042,12 +1037,9 @@
       <c r="F58" t="s">
         <v>7</v>
       </c>
-      <c r="I58" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D59" t="s">
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D59" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E59">
@@ -1056,178 +1048,141 @@
       <c r="F59" t="s">
         <v>39</v>
       </c>
-      <c r="I59" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D60" t="s">
+      <c r="H59" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D60" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E60">
+        <v>403</v>
+      </c>
+      <c r="F60" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D61" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E61">
         <v>204</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G61" t="s">
         <v>43</v>
       </c>
-      <c r="I60" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D61" t="s">
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D62" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D63" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D64" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G61" t="s">
-        <v>0</v>
-      </c>
-      <c r="I61" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D62" t="s">
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="G65" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G62" t="s">
-        <v>34</v>
-      </c>
-      <c r="I62" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D63" t="s">
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="G66" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G63" t="s">
-        <v>31</v>
-      </c>
-      <c r="I63" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D64" t="s">
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="G67" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G64" t="s">
-        <v>32</v>
-      </c>
-      <c r="I64" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="G65" t="s">
-        <v>33</v>
-      </c>
-      <c r="I65" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="G66" t="s">
-        <v>35</v>
-      </c>
-      <c r="I66" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="I67" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B68" t="s">
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B69" t="s">
         <v>24</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C69" t="s">
         <v>12</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D69" t="s">
         <v>40</v>
       </c>
-      <c r="E68">
+      <c r="E69" s="2">
         <v>404</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F69" t="s">
         <v>36</v>
-      </c>
-      <c r="I68" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D69" t="s">
-        <v>0</v>
-      </c>
-      <c r="E69">
-        <v>403</v>
-      </c>
-      <c r="F69" t="s">
-        <v>38</v>
-      </c>
-      <c r="I69" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D70" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E70">
+        <v>404</v>
+      </c>
+      <c r="F70" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="E71">
+        <v>403</v>
+      </c>
+      <c r="F71" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="E72">
+        <v>403</v>
+      </c>
+      <c r="F72" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="E73">
         <v>204</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F73" t="s">
         <v>37</v>
       </c>
-      <c r="I70" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="I71" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B72" t="s">
-        <v>3</v>
-      </c>
-      <c r="C72" t="s">
-        <v>42</v>
-      </c>
-      <c r="D72" t="s">
-        <v>0</v>
-      </c>
-      <c r="E72">
-        <v>200</v>
-      </c>
-      <c r="I72" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D73" t="s">
-        <v>34</v>
-      </c>
-      <c r="I73" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D74" t="s">
-        <v>31</v>
-      </c>
-      <c r="I74" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B75" t="s">
+        <v>24</v>
+      </c>
+      <c r="C75" t="s">
+        <v>23</v>
+      </c>
       <c r="D75" t="s">
-        <v>32</v>
+        <v>40</v>
+      </c>
+      <c r="E75" s="2">
+        <v>404</v>
+      </c>
+      <c r="F75" t="s">
+        <v>36</v>
+      </c>
+      <c r="H75" t="s">
+        <v>25</v>
       </c>
       <c r="I75" t="s">
         <v>28</v>
@@ -1235,22 +1190,120 @@
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D76" t="s">
+        <v>43</v>
+      </c>
+      <c r="E76">
+        <v>404</v>
+      </c>
+      <c r="F76" t="s">
+        <v>7</v>
+      </c>
+      <c r="I76" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="E77">
+        <v>403</v>
+      </c>
+      <c r="F77" t="s">
+        <v>39</v>
+      </c>
+      <c r="I77" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="E78">
+        <v>403</v>
+      </c>
+      <c r="F78" t="s">
+        <v>38</v>
+      </c>
+      <c r="I78" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="E79">
+        <v>204</v>
+      </c>
+      <c r="F79" t="s">
+        <v>37</v>
+      </c>
+      <c r="I79" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="I80" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="I81" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B82" t="s">
+        <v>3</v>
+      </c>
+      <c r="C82" t="s">
+        <v>42</v>
+      </c>
+      <c r="D82" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>200</v>
+      </c>
+      <c r="I82" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D83" t="s">
+        <v>34</v>
+      </c>
+      <c r="I83" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D84" t="s">
+        <v>31</v>
+      </c>
+      <c r="I84" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D85" t="s">
+        <v>32</v>
+      </c>
+      <c r="I85" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D86" t="s">
         <v>33</v>
       </c>
-      <c r="I76" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="D77" t="s">
+      <c r="I86" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D87" t="s">
         <v>35</v>
       </c>
-      <c r="I77" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="I78" t="s">
+      <c r="I87" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="I88" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Milestone 1 complete. Added authService, login with frontend works now.
</commit_message>
<xml_diff>
--- a/docs/Overwiew_endpoints.xlsx
+++ b/docs/Overwiew_endpoints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\ese2019-team8\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_UNI\ESE\ese2019-team8\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="13_ncr:1_{B5DC8251-7362-486E-BBB3-F9F8283E12C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1EFD8973-CDF8-4DE6-A7F4-79074428D0B8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31F38BC-0439-4D4F-B6D8-CEA2AF46B09C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -524,20 +524,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B759F60C-B498-4DED-A37F-801BD6AC74F2}">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>5</v>
       </c>
@@ -545,7 +547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -559,9 +561,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -576,7 +578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>1</v>
       </c>
@@ -587,7 +589,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6">
         <v>200</v>
       </c>
@@ -598,7 +600,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -615,7 +617,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>13</v>
       </c>
@@ -626,7 +628,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>1</v>
       </c>
@@ -637,7 +639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>14</v>
       </c>
@@ -645,7 +647,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>15</v>
       </c>
@@ -653,7 +655,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>16</v>
       </c>
@@ -661,7 +663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>17</v>
       </c>
@@ -669,7 +671,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>18</v>
       </c>
@@ -677,17 +679,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>3</v>
       </c>
@@ -704,7 +706,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E20">
         <v>200</v>
       </c>
@@ -712,42 +714,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>21</v>
       </c>
@@ -764,7 +766,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D30" s="1" t="s">
         <v>13</v>
       </c>
@@ -778,7 +780,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D31" s="1" t="s">
         <v>1</v>
       </c>
@@ -789,7 +791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D32" s="1" t="s">
         <v>14</v>
       </c>
@@ -797,7 +799,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D33" s="1" t="s">
         <v>15</v>
       </c>
@@ -805,7 +807,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D34" s="1" t="s">
         <v>16</v>
       </c>
@@ -813,7 +815,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D35" s="1" t="s">
         <v>17</v>
       </c>
@@ -821,7 +823,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D36" s="1" t="s">
         <v>18</v>
       </c>
@@ -829,12 +831,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G37" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>21</v>
       </c>
@@ -857,7 +859,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>20</v>
       </c>
@@ -871,12 +873,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>24</v>
       </c>
@@ -899,7 +901,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>0</v>
       </c>
@@ -913,12 +915,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I44" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -932,7 +934,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>10</v>
       </c>
@@ -949,7 +951,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>34</v>
       </c>
@@ -960,7 +962,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
         <v>31</v>
       </c>
@@ -971,7 +973,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
         <v>32</v>
       </c>
@@ -979,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
         <v>33</v>
       </c>
@@ -987,7 +989,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
         <v>35</v>
       </c>
@@ -995,22 +997,22 @@
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G53" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G54" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G55" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>21</v>
       </c>
@@ -1027,7 +1029,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
         <v>43</v>
       </c>
@@ -1038,7 +1040,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D59" s="1" t="s">
         <v>0</v>
       </c>
@@ -1052,7 +1054,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D60" s="1" t="s">
         <v>34</v>
       </c>
@@ -1063,7 +1065,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D61" s="1" t="s">
         <v>31</v>
       </c>
@@ -1074,7 +1076,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D62" s="1" t="s">
         <v>32</v>
       </c>
@@ -1082,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D63" s="1" t="s">
         <v>33</v>
       </c>
@@ -1090,7 +1092,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D64" s="1" t="s">
         <v>35</v>
       </c>
@@ -1098,22 +1100,22 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G65" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G66" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G67" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>24</v>
       </c>
@@ -1130,7 +1132,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
         <v>43</v>
       </c>
@@ -1141,7 +1143,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E71">
         <v>403</v>
       </c>
@@ -1149,7 +1151,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E72">
         <v>403</v>
       </c>
@@ -1157,7 +1159,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E73">
         <v>204</v>
       </c>
@@ -1165,7 +1167,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>24</v>
       </c>
@@ -1188,7 +1190,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
         <v>43</v>
       </c>
@@ -1202,7 +1204,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E77">
         <v>403</v>
       </c>
@@ -1213,7 +1215,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E78">
         <v>403</v>
       </c>
@@ -1224,7 +1226,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E79">
         <v>204</v>
       </c>
@@ -1235,17 +1237,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I80" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I81" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>3</v>
       </c>
@@ -1262,7 +1264,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D83" t="s">
         <v>34</v>
       </c>
@@ -1270,7 +1272,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D84" t="s">
         <v>31</v>
       </c>
@@ -1278,7 +1280,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D85" t="s">
         <v>32</v>
       </c>
@@ -1286,7 +1288,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D86" t="s">
         <v>33</v>
       </c>
@@ -1294,7 +1296,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D87" t="s">
         <v>35</v>
       </c>
@@ -1302,7 +1304,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I88" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
added admin functions (backend): * approve existing User * delete existing User * delete existing Service
</commit_message>
<xml_diff>
--- a/docs/Overwiew_endpoints.xlsx
+++ b/docs/Overwiew_endpoints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_UNI\ESE\ese2019-team8\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\ese2019-team8\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31F38BC-0439-4D4F-B6D8-CEA2AF46B09C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="114_{E268F7BF-38EE-4947-8672-E5C890E8F563}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F8F74D7C-B84A-4426-8013-7FD611C81BCD}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="46">
   <si>
     <t>username</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>user successfully disapproved</t>
+  </si>
+  <si>
+    <t>to be deleted</t>
   </si>
 </sst>
 </file>
@@ -522,24 +528,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B759F60C-B498-4DED-A37F-801BD6AC74F2}">
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.59765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D1" t="s">
         <v>5</v>
       </c>
@@ -547,7 +551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -560,8 +564,11 @@
       <c r="G2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -571,14 +578,14 @@
       <c r="D4" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>404</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D5" t="s">
         <v>1</v>
       </c>
@@ -589,7 +596,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E6">
         <v>200</v>
       </c>
@@ -600,7 +607,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -617,7 +624,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
         <v>13</v>
       </c>
@@ -628,7 +635,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D10" t="s">
         <v>1</v>
       </c>
@@ -639,7 +646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
         <v>14</v>
       </c>
@@ -647,7 +654,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
         <v>15</v>
       </c>
@@ -655,7 +662,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D13" t="s">
         <v>16</v>
       </c>
@@ -663,7 +670,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D14" t="s">
         <v>17</v>
       </c>
@@ -671,7 +678,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D15" t="s">
         <v>18</v>
       </c>
@@ -679,17 +686,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>3</v>
       </c>
@@ -706,7 +713,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
       <c r="E20">
         <v>200</v>
       </c>
@@ -714,42 +721,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>21</v>
       </c>
@@ -766,7 +773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D30" s="1" t="s">
         <v>13</v>
       </c>
@@ -780,7 +787,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D31" s="1" t="s">
         <v>1</v>
       </c>
@@ -791,7 +798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D32" s="1" t="s">
         <v>14</v>
       </c>
@@ -799,7 +806,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D33" s="1" t="s">
         <v>15</v>
       </c>
@@ -807,7 +814,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D34" s="1" t="s">
         <v>16</v>
       </c>
@@ -815,7 +822,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D35" s="1" t="s">
         <v>17</v>
       </c>
@@ -823,7 +830,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D36" s="1" t="s">
         <v>18</v>
       </c>
@@ -831,12 +838,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G37" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
         <v>21</v>
       </c>
@@ -855,457 +862,429 @@
       <c r="H39" t="s">
         <v>25</v>
       </c>
-      <c r="I39" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>403</v>
+      </c>
+      <c r="F40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D41" t="s">
         <v>20</v>
       </c>
-      <c r="E40">
-        <v>204</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="E41">
+        <v>200</v>
+      </c>
+      <c r="F41" t="s">
         <v>27</v>
       </c>
-      <c r="I40" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I41" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E42">
+        <v>200</v>
+      </c>
+      <c r="F42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B44" t="s">
         <v>24</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C44" t="s">
         <v>12</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D44" t="s">
         <v>40</v>
       </c>
-      <c r="E42">
+      <c r="E44">
         <v>404</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F44" t="s">
         <v>7</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H44" t="s">
         <v>25</v>
       </c>
-      <c r="I42" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D45" t="s">
         <v>0</v>
       </c>
-      <c r="E43">
-        <v>204</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="E45">
+        <v>200</v>
+      </c>
+      <c r="F45" t="s">
         <v>26</v>
       </c>
-      <c r="I43" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I44" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
         <v>29</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B47" t="s">
         <v>3</v>
-      </c>
-      <c r="C45" t="s">
-        <v>12</v>
-      </c>
-      <c r="G45" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>10</v>
       </c>
       <c r="C47" t="s">
         <v>12</v>
       </c>
-      <c r="D47" t="s">
+      <c r="G47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" t="s">
         <v>40</v>
       </c>
-      <c r="E47">
+      <c r="E49">
         <v>404</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F49" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D48" t="s">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D50" t="s">
         <v>34</v>
       </c>
-      <c r="E48">
+      <c r="E50">
         <v>403</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F50" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D49" t="s">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D51" t="s">
         <v>31</v>
       </c>
-      <c r="E49">
+      <c r="E51">
         <v>201</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G51" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D50" t="s">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D52" t="s">
         <v>32</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G52" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D53" t="s">
         <v>33</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G53" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D52" t="s">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D54" t="s">
         <v>35</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G54" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G53" t="s">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G55" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G54" t="s">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G56" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G55" t="s">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G57" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B59" t="s">
         <v>21</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C59" t="s">
         <v>12</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D59" t="s">
         <v>40</v>
       </c>
-      <c r="E57" s="2">
+      <c r="E59" s="2">
         <v>404</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F59" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D60" t="s">
         <v>43</v>
       </c>
-      <c r="E58">
+      <c r="E60">
         <v>404</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F60" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D59" s="1" t="s">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D61" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E59">
+      <c r="E61">
         <v>403</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F61" t="s">
         <v>39</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H61" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D60" s="1" t="s">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D62" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E60">
+      <c r="E62">
         <v>403</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F62" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D61" s="1" t="s">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D63" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E61">
-        <v>204</v>
-      </c>
-      <c r="G61" t="s">
+      <c r="E63">
+        <v>200</v>
+      </c>
+      <c r="G63" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D62" s="1" t="s">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D64" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G62" s="1" t="s">
+      <c r="G64" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D63" s="1" t="s">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D65" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G63" s="1" t="s">
+      <c r="G65" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D64" s="1" t="s">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D66" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G64" s="1" t="s">
+      <c r="G66" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G65" s="1" t="s">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G67" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G66" s="1" t="s">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G68" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G67" s="1" t="s">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G69" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B71" t="s">
         <v>24</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C71" t="s">
         <v>12</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D71" t="s">
         <v>40</v>
       </c>
-      <c r="E69" s="2">
+      <c r="E71" s="2">
         <v>404</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F71" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D70" t="s">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D72" t="s">
         <v>43</v>
       </c>
-      <c r="E70">
+      <c r="E72">
         <v>404</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F72" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E71">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E73">
         <v>403</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F73" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E72">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E74">
         <v>403</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F74" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E73">
-        <v>204</v>
-      </c>
-      <c r="F73" t="s">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E75">
+        <v>200</v>
+      </c>
+      <c r="F75" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B77" t="s">
         <v>24</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C77" t="s">
         <v>23</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D77" t="s">
         <v>40</v>
       </c>
-      <c r="E75" s="2">
+      <c r="E77" s="2">
         <v>404</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F77" t="s">
         <v>36</v>
       </c>
-      <c r="H75" t="s">
+      <c r="H77" t="s">
         <v>25</v>
       </c>
-      <c r="I75" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D76" t="s">
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D78" t="s">
         <v>43</v>
       </c>
-      <c r="E76">
+      <c r="E78">
         <v>404</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F78" t="s">
         <v>7</v>
       </c>
-      <c r="I76" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E77">
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E79">
         <v>403</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F79" t="s">
         <v>39</v>
       </c>
-      <c r="I77" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E78">
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E80">
         <v>403</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F80" t="s">
         <v>38</v>
       </c>
-      <c r="I78" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E79">
-        <v>204</v>
-      </c>
-      <c r="F79" t="s">
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="E81">
+        <v>200</v>
+      </c>
+      <c r="F81" t="s">
         <v>37</v>
       </c>
-      <c r="I79" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I80" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="I81" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B84" t="s">
         <v>3</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C84" t="s">
         <v>42</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D84" t="s">
         <v>0</v>
       </c>
-      <c r="E82">
+      <c r="E84">
         <v>200</v>
-      </c>
-      <c r="I82" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D83" t="s">
-        <v>34</v>
-      </c>
-      <c r="I83" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D84" t="s">
-        <v>31</v>
       </c>
       <c r="I84" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D85" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I85" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D86" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I86" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.45">
       <c r="D87" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I87" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D88" t="s">
+        <v>33</v>
+      </c>
       <c r="I88" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D89" t="s">
+        <v>35</v>
+      </c>
+      <c r="I89" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="I90" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
slightly changed GET profile method: request now doesn't have to have a body token sent as parameter
</commit_message>
<xml_diff>
--- a/docs/Overwiew_endpoints.xlsx
+++ b/docs/Overwiew_endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\ese2019-team8\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="114_{E268F7BF-38EE-4947-8672-E5C890E8F563}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F8F74D7C-B84A-4426-8013-7FD611C81BCD}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="114_{E268F7BF-38EE-4947-8672-E5C890E8F563}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{30E16E55-BCB3-4FA4-A685-DB6393A62549}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="47">
   <si>
     <t>username</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>to be deleted</t>
+  </si>
+  <si>
+    <t>/profile/:token</t>
   </si>
 </sst>
 </file>
@@ -701,10 +704,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E19">
         <v>403</v>

</xml_diff>

<commit_message>
added search Service (backend) (not completely implemented)
</commit_message>
<xml_diff>
--- a/docs/Overwiew_endpoints.xlsx
+++ b/docs/Overwiew_endpoints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninabaumgartner/WebstormProjects/ese2019-team8/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\ese2019-team8\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F4EF07-40DB-AE46-AB2B-81E2B31C8B42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="114_{39B5E667-9514-48E7-8B0E-B9721CAF3113}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1E6BD262-26EC-40B1-8C69-3F618ACEAB85}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2880" yWindow="460" windowWidth="19400" windowHeight="10400" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
+    <workbookView xWindow="0" yWindow="1328" windowWidth="14400" windowHeight="7372" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="52">
   <si>
     <t>username</t>
   </si>
@@ -169,6 +169,24 @@
   </si>
   <si>
     <t>/profile/:token</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>User is not approved</t>
+  </si>
+  <si>
+    <t>Registration successful</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>priceMin</t>
+  </si>
+  <si>
+    <t>priceMax</t>
   </si>
 </sst>
 </file>
@@ -184,7 +202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +212,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -210,10 +234,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -528,24 +553,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B759F60C-B498-4DED-A37F-801BD6AC74F2}">
-  <dimension ref="A1:H89"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="I84" sqref="I84:I90"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D1" t="s">
         <v>5</v>
       </c>
@@ -553,7 +578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -570,7 +595,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -587,7 +612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D5" t="s">
         <v>1</v>
       </c>
@@ -598,7 +623,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E6">
         <v>200</v>
       </c>
@@ -609,7 +634,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -626,7 +651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
         <v>13</v>
       </c>
@@ -637,18 +662,21 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D10" t="s">
         <v>1</v>
       </c>
       <c r="E10">
         <v>201</v>
       </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
       <c r="G10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
         <v>14</v>
       </c>
@@ -656,7 +684,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
         <v>15</v>
       </c>
@@ -664,7 +692,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D13" t="s">
         <v>16</v>
       </c>
@@ -672,7 +700,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D14" t="s">
         <v>17</v>
       </c>
@@ -680,7 +708,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D15" t="s">
         <v>18</v>
       </c>
@@ -688,579 +716,626 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>3</v>
       </c>
       <c r="C19" t="s">
         <v>45</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
+        <v>404</v>
+      </c>
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E20">
         <v>403</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="E20">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E21">
         <v>200</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G21" t="s">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G22" t="s">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G23" t="s">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G24" t="s">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G25" t="s">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G26" t="s">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G27" t="s">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G28" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
         <v>21</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>22</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E30" s="2">
         <v>404</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F30" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D30" s="1" t="s">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D31" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E30">
+      <c r="E31">
         <v>403</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F31" t="s">
         <v>37</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D31" s="1" t="s">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D32" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <v>200</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G32" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D32" s="1" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D33" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D33" s="1" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D34" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D34" s="1" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D35" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D35" s="1" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D36" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D36" s="1" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D37" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G37" s="1" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G38" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B40" t="s">
         <v>21</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>23</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>39</v>
       </c>
-      <c r="E39">
+      <c r="E40">
         <v>404</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F40" t="s">
         <v>7</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H40" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D40" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D41" t="s">
         <v>0</v>
       </c>
-      <c r="E40">
+      <c r="E41">
         <v>403</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D41" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D42" t="s">
         <v>20</v>
       </c>
-      <c r="E41">
-        <v>200</v>
-      </c>
-      <c r="F41" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E42">
         <v>200</v>
       </c>
       <c r="F42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E43">
+        <v>200</v>
+      </c>
+      <c r="F43" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B45" t="s">
         <v>24</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>12</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>39</v>
       </c>
-      <c r="E44">
+      <c r="E45">
         <v>404</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F45" t="s">
         <v>7</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H45" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D45" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D46" t="s">
         <v>0</v>
       </c>
-      <c r="E45">
+      <c r="E46">
         <v>200</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F46" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
         <v>28</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>3</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>12</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G48" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B50" t="s">
         <v>10</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>12</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>39</v>
       </c>
-      <c r="E49">
+      <c r="E50">
         <v>404</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D50" t="s">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D51" t="s">
         <v>33</v>
       </c>
-      <c r="E50">
+      <c r="E51">
         <v>403</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F51" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D51" t="s">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D52" t="s">
         <v>30</v>
       </c>
-      <c r="E51">
+      <c r="E52">
+        <v>403</v>
+      </c>
+      <c r="F52" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D53" t="s">
+        <v>31</v>
+      </c>
+      <c r="E53">
         <v>201</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G53" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D52" t="s">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D54" t="s">
+        <v>32</v>
+      </c>
+      <c r="G54" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D55" t="s">
+        <v>34</v>
+      </c>
+      <c r="G55" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G56" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G57" t="s">
         <v>31</v>
       </c>
-      <c r="G52" t="s">
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G58" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G59" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B61" t="s">
+        <v>21</v>
+      </c>
+      <c r="C61" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" t="s">
+        <v>39</v>
+      </c>
+      <c r="E61" s="2">
+        <v>404</v>
+      </c>
+      <c r="F61" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D62" t="s">
+        <v>42</v>
+      </c>
+      <c r="E62">
+        <v>404</v>
+      </c>
+      <c r="F62" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D63" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D53" t="s">
+      <c r="E63">
+        <v>403</v>
+      </c>
+      <c r="F63" t="s">
+        <v>38</v>
+      </c>
+      <c r="H63" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D64" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E64">
+        <v>403</v>
+      </c>
+      <c r="F64" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D65" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E65">
+        <v>200</v>
+      </c>
+      <c r="G65" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D66" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D67" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G67" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D54" t="s">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D68" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G68" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G55" t="s">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G69" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G56" t="s">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G70" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G57" t="s">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G71" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
-        <v>21</v>
-      </c>
-      <c r="C59" t="s">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B73" t="s">
+        <v>24</v>
+      </c>
+      <c r="C73" t="s">
         <v>12</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D73" t="s">
         <v>39</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E73" s="2">
         <v>404</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F73" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D60" t="s">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D74" t="s">
         <v>42</v>
       </c>
-      <c r="E60">
+      <c r="E74">
         <v>404</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F74" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D61" s="1" t="s">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E75">
+        <v>403</v>
+      </c>
+      <c r="F75" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E76">
+        <v>403</v>
+      </c>
+      <c r="F76" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E77">
+        <v>200</v>
+      </c>
+      <c r="F77" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B79" t="s">
+        <v>24</v>
+      </c>
+      <c r="C79" t="s">
+        <v>23</v>
+      </c>
+      <c r="D79" t="s">
+        <v>39</v>
+      </c>
+      <c r="E79" s="2">
+        <v>404</v>
+      </c>
+      <c r="F79" t="s">
+        <v>35</v>
+      </c>
+      <c r="H79" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D80" t="s">
+        <v>42</v>
+      </c>
+      <c r="E80">
+        <v>404</v>
+      </c>
+      <c r="F80" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="E81">
+        <v>403</v>
+      </c>
+      <c r="F81" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="E82">
+        <v>403</v>
+      </c>
+      <c r="F82" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="E83">
+        <v>200</v>
+      </c>
+      <c r="F83" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B86" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" t="s">
+        <v>41</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E86">
+        <v>200</v>
+      </c>
+      <c r="I86" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D87" t="s">
         <v>0</v>
       </c>
-      <c r="E61">
-        <v>403</v>
-      </c>
-      <c r="F61" t="s">
-        <v>38</v>
-      </c>
-      <c r="H61" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D62" s="1" t="s">
+      <c r="I87" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D88" t="s">
         <v>33</v>
       </c>
-      <c r="E62">
-        <v>403</v>
-      </c>
-      <c r="F62" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D63" s="1" t="s">
+      <c r="I88" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D89" t="s">
         <v>30</v>
       </c>
-      <c r="E63">
-        <v>200</v>
-      </c>
-      <c r="G63" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D64" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D65" s="1" t="s">
+      <c r="I89" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D90" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I90" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D91" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I91" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D92" t="s">
         <v>32</v>
       </c>
-      <c r="G65" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D66" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G67" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G68" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G69" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B71" t="s">
-        <v>24</v>
-      </c>
-      <c r="C71" t="s">
-        <v>12</v>
-      </c>
-      <c r="D71" t="s">
-        <v>39</v>
-      </c>
-      <c r="E71" s="2">
-        <v>404</v>
-      </c>
-      <c r="F71" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D72" t="s">
-        <v>42</v>
-      </c>
-      <c r="E72">
-        <v>404</v>
-      </c>
-      <c r="F72" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="E73">
-        <v>403</v>
-      </c>
-      <c r="F73" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="E74">
-        <v>403</v>
-      </c>
-      <c r="F74" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="E75">
-        <v>200</v>
-      </c>
-      <c r="F75" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B77" t="s">
-        <v>24</v>
-      </c>
-      <c r="C77" t="s">
-        <v>23</v>
-      </c>
-      <c r="D77" t="s">
-        <v>39</v>
-      </c>
-      <c r="E77" s="2">
-        <v>404</v>
-      </c>
-      <c r="F77" t="s">
-        <v>35</v>
-      </c>
-      <c r="H77" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D78" t="s">
-        <v>42</v>
-      </c>
-      <c r="E78">
-        <v>404</v>
-      </c>
-      <c r="F78" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="E79">
-        <v>403</v>
-      </c>
-      <c r="F79" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="E80">
-        <v>403</v>
-      </c>
-      <c r="F80" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E81">
-        <v>200</v>
-      </c>
-      <c r="F81" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B84" t="s">
-        <v>3</v>
-      </c>
-      <c r="C84" t="s">
-        <v>41</v>
-      </c>
-      <c r="D84" t="s">
-        <v>0</v>
-      </c>
-      <c r="E84">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D85" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D86" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D87" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D88" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D89" t="s">
+      <c r="I92" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="D93" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Simplified registration form. Removed all toDoItem and toDoList stuff. Removed unused files.
</commit_message>
<xml_diff>
--- a/docs/Overwiew_endpoints.xlsx
+++ b/docs/Overwiew_endpoints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninabaumgartner/WebstormProjects/ese2019-team8/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_UNI\ESE\ese2019-team8\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F4EF07-40DB-AE46-AB2B-81E2B31C8B42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A73B695-83C6-489E-9A1F-F6DC427C5DDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2880" yWindow="460" windowWidth="19400" windowHeight="10400" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
+    <workbookView xWindow="5400" yWindow="-18120" windowWidth="29040" windowHeight="17640" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="47">
   <si>
     <t>username</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>/profile/:token</t>
+  </si>
+  <si>
+    <t>konkret: localhost:3000/profile/sldkdvsokegerwngoiwrejg9803w4gi34go34o348whgo43g3go823</t>
   </si>
 </sst>
 </file>
@@ -216,7 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -232,7 +235,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -530,22 +533,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B759F60C-B498-4DED-A37F-801BD6AC74F2}">
   <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="I84" sqref="I84:I90"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D1" t="s">
         <v>5</v>
       </c>
@@ -553,7 +556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -570,7 +573,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -587,7 +590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D5" t="s">
         <v>1</v>
       </c>
@@ -598,7 +601,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E6">
         <v>200</v>
       </c>
@@ -609,7 +612,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -626,7 +629,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
         <v>13</v>
       </c>
@@ -637,7 +640,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D10" t="s">
         <v>1</v>
       </c>
@@ -648,7 +651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
         <v>14</v>
       </c>
@@ -656,7 +659,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
         <v>15</v>
       </c>
@@ -664,7 +667,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D13" t="s">
         <v>16</v>
       </c>
@@ -672,7 +675,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D14" t="s">
         <v>17</v>
       </c>
@@ -680,7 +683,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D15" t="s">
         <v>18</v>
       </c>
@@ -688,17 +691,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>3</v>
       </c>
@@ -711,8 +714,11 @@
       <c r="F19" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
       <c r="E20">
         <v>200</v>
       </c>
@@ -720,42 +726,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>21</v>
       </c>
@@ -772,7 +778,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D30" s="1" t="s">
         <v>13</v>
       </c>
@@ -786,7 +792,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D31" s="1" t="s">
         <v>1</v>
       </c>
@@ -797,7 +803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D32" s="1" t="s">
         <v>14</v>
       </c>
@@ -805,7 +811,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D33" s="1" t="s">
         <v>15</v>
       </c>
@@ -813,7 +819,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D34" s="1" t="s">
         <v>16</v>
       </c>
@@ -821,7 +827,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D35" s="1" t="s">
         <v>17</v>
       </c>
@@ -829,7 +835,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D36" s="1" t="s">
         <v>18</v>
       </c>
@@ -837,12 +843,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G37" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
         <v>21</v>
       </c>
@@ -862,7 +868,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D40" t="s">
         <v>0</v>
       </c>
@@ -873,7 +879,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D41" t="s">
         <v>20</v>
       </c>
@@ -884,7 +890,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E42">
         <v>200</v>
       </c>
@@ -892,7 +898,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
         <v>24</v>
       </c>
@@ -912,7 +918,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D45" t="s">
         <v>0</v>
       </c>
@@ -923,7 +929,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>28</v>
       </c>
@@ -937,7 +943,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B49" t="s">
         <v>10</v>
       </c>
@@ -954,7 +960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D50" t="s">
         <v>33</v>
       </c>
@@ -965,7 +971,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D51" t="s">
         <v>30</v>
       </c>
@@ -976,7 +982,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D52" t="s">
         <v>31</v>
       </c>
@@ -984,7 +990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D53" t="s">
         <v>32</v>
       </c>
@@ -992,7 +998,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D54" t="s">
         <v>34</v>
       </c>
@@ -1000,22 +1006,22 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G55" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G56" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G57" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B59" t="s">
         <v>21</v>
       </c>
@@ -1032,7 +1038,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D60" t="s">
         <v>42</v>
       </c>
@@ -1043,7 +1049,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D61" s="1" t="s">
         <v>0</v>
       </c>
@@ -1057,7 +1063,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D62" s="1" t="s">
         <v>33</v>
       </c>
@@ -1068,7 +1074,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D63" s="1" t="s">
         <v>30</v>
       </c>
@@ -1079,7 +1085,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D64" s="1" t="s">
         <v>31</v>
       </c>
@@ -1087,7 +1093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D65" s="1" t="s">
         <v>32</v>
       </c>
@@ -1095,7 +1101,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D66" s="1" t="s">
         <v>34</v>
       </c>
@@ -1103,22 +1109,22 @@
         <v>30</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G67" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G68" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G69" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B71" t="s">
         <v>24</v>
       </c>
@@ -1135,7 +1141,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D72" t="s">
         <v>42</v>
       </c>
@@ -1146,7 +1152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.45">
       <c r="E73">
         <v>403</v>
       </c>
@@ -1154,7 +1160,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.45">
       <c r="E74">
         <v>403</v>
       </c>
@@ -1162,7 +1168,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.45">
       <c r="E75">
         <v>200</v>
       </c>
@@ -1170,7 +1176,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B77" t="s">
         <v>24</v>
       </c>
@@ -1190,7 +1196,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D78" t="s">
         <v>42</v>
       </c>
@@ -1201,7 +1207,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.45">
       <c r="E79">
         <v>403</v>
       </c>
@@ -1209,7 +1215,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.45">
       <c r="E80">
         <v>403</v>
       </c>
@@ -1217,7 +1223,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.45">
       <c r="E81">
         <v>200</v>
       </c>
@@ -1225,7 +1231,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B84" t="s">
         <v>3</v>
       </c>
@@ -1239,27 +1245,27 @@
         <v>200</v>
       </c>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D85" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D86" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D87" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D88" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D89" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
* added documentation for most of the methods (backend) * added explicit preconditions for POST methods * added check, if isServiceProvider, for creating Services * deleted unused, commented method (@user.controller.ts) * found bug when deleting existing User with existing Services (added TODO)
</commit_message>
<xml_diff>
--- a/docs/Overwiew_endpoints.xlsx
+++ b/docs/Overwiew_endpoints.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_UNI\ESE\ese2019-team8\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\ese2019-team8\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A73B695-83C6-489E-9A1F-F6DC427C5DDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="114_{370FD315-8FA4-4C58-8A8E-74881233F0BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3B0D1DF0-2615-4255-9AF8-A20F9213D0C7}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="-18120" windowWidth="29040" windowHeight="17640" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="52">
   <si>
     <t>username</t>
   </si>
@@ -172,6 +172,21 @@
   </si>
   <si>
     <t>konkret: localhost:3000/profile/sldkdvsokegerwngoiwrejg9803w4gi34go34o348whgo43g3go823</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>priceMin</t>
+  </si>
+  <si>
+    <t>priceMax</t>
+  </si>
+  <si>
+    <t>blau = verpfllichtend</t>
+  </si>
+  <si>
+    <t>precondition failed</t>
   </si>
 </sst>
 </file>
@@ -187,7 +202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,6 +212,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -213,13 +240,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -235,7 +264,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -531,13 +560,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B759F60C-B498-4DED-A37F-801BD6AC74F2}">
-  <dimension ref="A1:H89"/>
+  <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="8.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.1328125" bestFit="1" customWidth="1"/>
@@ -619,44 +646,50 @@
       <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="2">
-        <v>404</v>
+      <c r="E8">
+        <v>413</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>51</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
+        <v>404</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10">
         <v>403</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>201</v>
-      </c>
-      <c r="G10" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
         <v>14</v>
       </c>
+      <c r="E11">
+        <v>201</v>
+      </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
@@ -664,7 +697,7 @@
         <v>15</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
@@ -672,7 +705,7 @@
         <v>16</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
@@ -680,7 +713,7 @@
         <v>17</v>
       </c>
       <c r="G14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
@@ -688,585 +721,611 @@
         <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B19" t="s">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
         <v>3</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>45</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>403</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>38</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E20">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E21">
         <v>200</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G21" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G28" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B29" t="s">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
         <v>21</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>22</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E30" s="2">
         <v>404</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F30" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30">
-        <v>403</v>
-      </c>
-      <c r="F30" t="s">
-        <v>37</v>
-      </c>
-      <c r="H30" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D31" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E31">
-        <v>200</v>
-      </c>
-      <c r="G31" t="s">
-        <v>0</v>
+        <v>403</v>
+      </c>
+      <c r="F31" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>200</v>
+      </c>
+      <c r="G32" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D33" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D34" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D35" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D37" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G37" s="1" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G38" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B39" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B40" t="s">
         <v>21</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>23</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>39</v>
       </c>
-      <c r="E39">
+      <c r="E40">
         <v>404</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F40" t="s">
         <v>7</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H40" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D40" t="s">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>403</v>
-      </c>
-      <c r="F40" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>403</v>
+      </c>
+      <c r="F41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D42" t="s">
         <v>20</v>
       </c>
-      <c r="E41">
-        <v>200</v>
-      </c>
-      <c r="F41" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E42">
         <v>200</v>
       </c>
       <c r="F42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E43">
+        <v>200</v>
+      </c>
+      <c r="F43" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B44" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B45" t="s">
         <v>24</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>12</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>39</v>
       </c>
-      <c r="E44">
+      <c r="E45">
         <v>404</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F45" t="s">
         <v>7</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H45" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D45" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D46" t="s">
         <v>0</v>
       </c>
-      <c r="E45">
+      <c r="E46">
         <v>200</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F46" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
         <v>28</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>3</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>12</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G48" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B49" t="s">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B50" t="s">
         <v>10</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>12</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>39</v>
       </c>
-      <c r="E49">
+      <c r="E50">
+        <v>413</v>
+      </c>
+      <c r="F50" t="s">
+        <v>51</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D51" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E51">
         <v>404</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F51" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D50" t="s">
-        <v>33</v>
-      </c>
-      <c r="E50">
-        <v>403</v>
-      </c>
-      <c r="F50" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D51" t="s">
-        <v>30</v>
-      </c>
-      <c r="E51">
-        <v>201</v>
-      </c>
-      <c r="G51" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D52" t="s">
-        <v>31</v>
-      </c>
-      <c r="G52" t="s">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="E52">
+        <v>403</v>
+      </c>
+      <c r="F52" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D53" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="E53">
+        <v>201</v>
       </c>
       <c r="G53" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D54" t="s">
+        <v>32</v>
+      </c>
+      <c r="G54" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D55" t="s">
         <v>34</v>
       </c>
-      <c r="G54" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G55" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G56" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G57" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G58" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G59" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B59" t="s">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B61" t="s">
         <v>21</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C61" t="s">
         <v>12</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D61" t="s">
         <v>39</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E61" s="2">
         <v>404</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F61" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D60" t="s">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D62" t="s">
         <v>42</v>
       </c>
-      <c r="E60">
+      <c r="E62">
         <v>404</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F62" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D61" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E61">
-        <v>403</v>
-      </c>
-      <c r="F61" t="s">
-        <v>38</v>
-      </c>
-      <c r="H61" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D62" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E62">
-        <v>403</v>
-      </c>
-      <c r="F62" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D63" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E63">
-        <v>200</v>
-      </c>
-      <c r="G63" t="s">
-        <v>42</v>
+        <v>403</v>
+      </c>
+      <c r="F63" t="s">
+        <v>38</v>
+      </c>
+      <c r="H63" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D64" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="E64">
+        <v>403</v>
+      </c>
+      <c r="F64" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D65" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="E65">
+        <v>200</v>
+      </c>
+      <c r="G65" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D66" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D67" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D68" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G66" s="1" t="s">
+      <c r="G68" s="1" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G67" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G68" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G69" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G70" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G71" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B71" t="s">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B73" t="s">
         <v>24</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C73" t="s">
         <v>12</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D73" t="s">
         <v>39</v>
       </c>
-      <c r="E71" s="2">
+      <c r="E73" s="2">
         <v>404</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F73" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D72" t="s">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D74" t="s">
         <v>42</v>
       </c>
-      <c r="E72">
+      <c r="E74">
         <v>404</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F74" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E73">
-        <v>403</v>
-      </c>
-      <c r="F73" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E74">
-        <v>403</v>
-      </c>
-      <c r="F74" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.45">
       <c r="E75">
+        <v>403</v>
+      </c>
+      <c r="F75" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E76">
+        <v>403</v>
+      </c>
+      <c r="F76" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E77">
         <v>200</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F77" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B77" t="s">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B79" t="s">
         <v>24</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C79" t="s">
         <v>23</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D79" t="s">
         <v>39</v>
       </c>
-      <c r="E77" s="2">
+      <c r="E79" s="2">
         <v>404</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F79" t="s">
         <v>35</v>
       </c>
-      <c r="H77" t="s">
+      <c r="H79" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D78" t="s">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D80" t="s">
         <v>42</v>
       </c>
-      <c r="E78">
+      <c r="E80">
         <v>404</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F80" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E79">
-        <v>403</v>
-      </c>
-      <c r="F79" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E80">
-        <v>403</v>
-      </c>
-      <c r="F80" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.45">
       <c r="E81">
+        <v>403</v>
+      </c>
+      <c r="F81" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="E82">
+        <v>403</v>
+      </c>
+      <c r="F82" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="E83">
         <v>200</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F83" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B84" t="s">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B86" t="s">
         <v>3</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C86" t="s">
         <v>41</v>
       </c>
-      <c r="D84" t="s">
-        <v>0</v>
-      </c>
-      <c r="E84">
+      <c r="D86" t="s">
+        <v>47</v>
+      </c>
+      <c r="E86">
         <v>200</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="D85" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="D86" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D87" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D88" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D89" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="D90" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="D91" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="D92" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="D93" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added DELETE user by user (backend) changed path of DELETE user by admin (backend)
</commit_message>
<xml_diff>
--- a/docs/Overwiew_endpoints.xlsx
+++ b/docs/Overwiew_endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\ese2019-team8\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="114_{370FD315-8FA4-4C58-8A8E-74881233F0BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3B0D1DF0-2615-4255-9AF8-A20F9213D0C7}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="114_{370FD315-8FA4-4C58-8A8E-74881233F0BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{29C5E8FA-1525-4E5F-B485-CF66DB268DA0}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="52">
   <si>
     <t>username</t>
   </si>
@@ -560,7 +560,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B759F60C-B498-4DED-A37F-801BD6AC74F2}">
-  <dimension ref="A1:H93"/>
+  <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -841,7 +841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D33" s="1" t="s">
         <v>14</v>
       </c>
@@ -849,7 +849,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D34" s="1" t="s">
         <v>15</v>
       </c>
@@ -857,7 +857,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D35" s="1" t="s">
         <v>16</v>
       </c>
@@ -865,7 +865,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D36" s="1" t="s">
         <v>17</v>
       </c>
@@ -873,7 +873,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D37" s="1" t="s">
         <v>18</v>
       </c>
@@ -881,17 +881,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G38" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D40" t="s">
         <v>39</v>
@@ -902,430 +902,471 @@
       <c r="F40" t="s">
         <v>7</v>
       </c>
-      <c r="H40" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D41" t="s">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.45">
       <c r="E41">
         <v>403</v>
       </c>
       <c r="F41" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D42" t="s">
-        <v>20</v>
-      </c>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.45">
       <c r="E42">
         <v>200</v>
       </c>
       <c r="F42" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="E43">
-        <v>200</v>
-      </c>
-      <c r="F43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B45" t="s">
-        <v>24</v>
-      </c>
-      <c r="C45" t="s">
-        <v>12</v>
-      </c>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B44" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" t="s">
+        <v>39</v>
+      </c>
+      <c r="E44">
+        <v>404</v>
+      </c>
+      <c r="F44" t="s">
+        <v>7</v>
+      </c>
+      <c r="H44" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D45" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F45" t="s">
-        <v>7</v>
-      </c>
-      <c r="H45" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D46" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E46">
         <v>200</v>
       </c>
       <c r="F46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E47">
+        <v>200</v>
+      </c>
+      <c r="F47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B49" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" t="s">
+        <v>39</v>
+      </c>
+      <c r="E49">
+        <v>404</v>
+      </c>
+      <c r="F49" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D50" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>403</v>
+      </c>
+      <c r="F50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E51">
+        <v>200</v>
+      </c>
+      <c r="F51" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
         <v>28</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B53" t="s">
         <v>3</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C53" t="s">
         <v>12</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G53" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B50" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B55" t="s">
         <v>10</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C55" t="s">
         <v>12</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D55" t="s">
         <v>39</v>
       </c>
-      <c r="E50">
+      <c r="E55">
         <v>413</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F55" t="s">
         <v>51</v>
       </c>
-      <c r="H50" s="4" t="s">
+      <c r="H55" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D51" s="4" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D56" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E51">
+      <c r="E56">
         <v>404</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F56" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D52" t="s">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D57" t="s">
         <v>30</v>
       </c>
-      <c r="E52">
+      <c r="E57">
         <v>403</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F57" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D53" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D58" t="s">
         <v>31</v>
       </c>
-      <c r="E53">
+      <c r="E58">
         <v>201</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G58" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D54" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D59" t="s">
         <v>32</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G59" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D55" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D60" t="s">
         <v>34</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G60" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G56" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G61" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G57" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G62" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G58" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G63" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G59" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G64" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B61" t="s">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B66" t="s">
         <v>21</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C66" t="s">
         <v>12</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D66" t="s">
         <v>39</v>
       </c>
-      <c r="E61" s="2">
+      <c r="E66" s="2">
         <v>404</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F66" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D62" t="s">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D67" t="s">
         <v>42</v>
       </c>
-      <c r="E62">
+      <c r="E67">
         <v>404</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F67" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D63" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E63">
-        <v>403</v>
-      </c>
-      <c r="F63" t="s">
-        <v>38</v>
-      </c>
-      <c r="H63" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D64" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E64">
-        <v>403</v>
-      </c>
-      <c r="F64" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D65" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E65">
-        <v>200</v>
-      </c>
-      <c r="G65" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D66" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D67" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>403</v>
+      </c>
+      <c r="F68" t="s">
+        <v>38</v>
+      </c>
+      <c r="H68" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D69" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E69">
+        <v>403</v>
+      </c>
+      <c r="F69" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D70" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E70">
+        <v>200</v>
+      </c>
+      <c r="G70" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D71" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D72" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D73" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G68" s="1" t="s">
+      <c r="G73" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G69" s="1" t="s">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G74" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G70" s="1" t="s">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G75" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G71" s="1" t="s">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G76" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B73" t="s">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B78" t="s">
         <v>24</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C78" t="s">
         <v>12</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D78" t="s">
         <v>39</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E78" s="2">
         <v>404</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F78" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D74" t="s">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D79" t="s">
         <v>42</v>
       </c>
-      <c r="E74">
+      <c r="E79">
         <v>404</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F79" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E75">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E80">
         <v>403</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F80" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E76">
-        <v>403</v>
-      </c>
-      <c r="F76" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E77">
-        <v>200</v>
-      </c>
-      <c r="F77" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B79" t="s">
-        <v>24</v>
-      </c>
-      <c r="C79" t="s">
-        <v>23</v>
-      </c>
-      <c r="D79" t="s">
-        <v>39</v>
-      </c>
-      <c r="E79" s="2">
-        <v>404</v>
-      </c>
-      <c r="F79" t="s">
-        <v>35</v>
-      </c>
-      <c r="H79" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D80" t="s">
-        <v>42</v>
-      </c>
-      <c r="E80">
-        <v>404</v>
-      </c>
-      <c r="F80" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.45">
       <c r="E81">
         <v>403</v>
       </c>
       <c r="F81" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E82">
+        <v>200</v>
+      </c>
+      <c r="F82" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B84" t="s">
+        <v>24</v>
+      </c>
+      <c r="C84" t="s">
+        <v>23</v>
+      </c>
+      <c r="D84" t="s">
+        <v>39</v>
+      </c>
+      <c r="E84" s="2">
+        <v>404</v>
+      </c>
+      <c r="F84" t="s">
+        <v>35</v>
+      </c>
+      <c r="H84" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D85" t="s">
+        <v>42</v>
+      </c>
+      <c r="E85">
+        <v>404</v>
+      </c>
+      <c r="F85" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E86">
+        <v>403</v>
+      </c>
+      <c r="F86" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="E82">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E87">
         <v>403</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F87" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="E83">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E88">
         <v>200</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F88" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B86" t="s">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B91" t="s">
         <v>3</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C91" t="s">
         <v>41</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D91" t="s">
         <v>47</v>
       </c>
-      <c r="E86">
+      <c r="E91">
         <v>200</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="D87" t="s">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D92" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="D88" t="s">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D93" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="D89" t="s">
+    <row r="94" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D94" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="D90" s="3" t="s">
+    <row r="95" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D95" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="D91" s="3" t="s">
+    <row r="96" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D96" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="D92" t="s">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D97" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="D93" t="s">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D98" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added GET all Users function (backend)
</commit_message>
<xml_diff>
--- a/docs/Overwiew_endpoints.xlsx
+++ b/docs/Overwiew_endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\ese2019-team8\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="114_{370FD315-8FA4-4C58-8A8E-74881233F0BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{29C5E8FA-1525-4E5F-B485-CF66DB268DA0}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="114_{370FD315-8FA4-4C58-8A8E-74881233F0BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3394C93D-52CB-43E7-8479-323B014CC8C5}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="57">
   <si>
     <t>username</t>
   </si>
@@ -165,9 +165,6 @@
     <t>user successfully disapproved</t>
   </si>
   <si>
-    <t>to be deleted</t>
-  </si>
-  <si>
     <t>/profile/:token</t>
   </si>
   <si>
@@ -187,6 +184,24 @@
   </si>
   <si>
     <t>precondition failed</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>/allUsers/:token</t>
+  </si>
+  <si>
+    <t>(token oder username)</t>
+  </si>
+  <si>
+    <t>(!isServiceProvider)</t>
+  </si>
+  <si>
+    <t>not approved</t>
+  </si>
+  <si>
+    <t>Array aller passender Services</t>
   </si>
 </sst>
 </file>
@@ -560,7 +575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B759F60C-B498-4DED-A37F-801BD6AC74F2}">
-  <dimension ref="A1:H98"/>
+  <dimension ref="A1:K104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -591,413 +606,412 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2">
+        <v>404</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E3">
+        <v>403</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E4">
+        <v>403</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E5">
+        <v>200</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>404</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>403</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E9">
+        <v>200</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="2">
-        <v>404</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>403</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="E6">
-        <v>200</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8">
+      <c r="E11">
         <v>413</v>
       </c>
-      <c r="F8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="F11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="2">
-        <v>404</v>
-      </c>
-      <c r="F9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>403</v>
-      </c>
-      <c r="F10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11">
-        <v>201</v>
-      </c>
-      <c r="G11" t="s">
-        <v>0</v>
+      <c r="H11" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" t="s">
         <v>13</v>
       </c>
+      <c r="E12">
+        <v>403</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D13" t="s">
-        <v>16</v>
+      <c r="D13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>201</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D18" t="s">
         <v>18</v>
       </c>
-      <c r="G15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G16" t="s">
+      <c r="G18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G17" t="s">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G18" t="s">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B20" t="s">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
         <v>3</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="2">
+        <v>404</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" t="s">
         <v>45</v>
       </c>
-      <c r="E20">
-        <v>403</v>
-      </c>
-      <c r="F20" t="s">
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E23">
+        <v>403</v>
+      </c>
+      <c r="F23" t="s">
         <v>38</v>
       </c>
-      <c r="H20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E21">
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E24">
         <v>200</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G24" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G24" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G25" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G26" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G27" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G31" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B30" t="s">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
         <v>21</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C33" t="s">
         <v>22</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D33" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E33" s="2">
         <v>404</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F33" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31">
-        <v>403</v>
-      </c>
-      <c r="F31" t="s">
-        <v>37</v>
-      </c>
-      <c r="H31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <v>200</v>
-      </c>
-      <c r="G32" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="E34">
+        <v>403</v>
+      </c>
+      <c r="F34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H34" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D35" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>15</v>
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>200</v>
+      </c>
+      <c r="G35" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D36" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D40" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G38" s="1" t="s">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G41" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B40" t="s">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B43" t="s">
         <v>24</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C43" t="s">
         <v>22</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D43" t="s">
         <v>39</v>
       </c>
-      <c r="E40">
+      <c r="E43">
         <v>404</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F43" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E41">
-        <v>403</v>
-      </c>
-      <c r="F41" t="s">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E44">
+        <v>403</v>
+      </c>
+      <c r="F44" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E42">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E45">
         <v>200</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F45" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B44" t="s">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B47" t="s">
         <v>21</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C47" t="s">
         <v>23</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D47" t="s">
         <v>39</v>
       </c>
-      <c r="E44">
+      <c r="E47">
         <v>404</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F47" t="s">
         <v>7</v>
       </c>
-      <c r="H44" t="s">
+      <c r="G47" t="s">
+        <v>53</v>
+      </c>
+      <c r="H47" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D45" t="s">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D48" t="s">
         <v>0</v>
       </c>
-      <c r="E45">
-        <v>403</v>
-      </c>
-      <c r="F45" t="s">
+      <c r="E48">
+        <v>403</v>
+      </c>
+      <c r="F48" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49">
+        <v>403</v>
+      </c>
+      <c r="F49" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D46" t="s">
-        <v>20</v>
-      </c>
-      <c r="E46">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E50">
         <v>200</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F50" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E47">
-        <v>200</v>
-      </c>
-      <c r="F47" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B49" t="s">
-        <v>24</v>
-      </c>
-      <c r="C49" t="s">
-        <v>23</v>
-      </c>
-      <c r="D49" t="s">
-        <v>39</v>
-      </c>
-      <c r="E49">
-        <v>404</v>
-      </c>
-      <c r="F49" t="s">
-        <v>7</v>
-      </c>
-      <c r="H49" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D50" t="s">
-        <v>0</v>
-      </c>
-      <c r="E50">
-        <v>403</v>
-      </c>
-      <c r="F50" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.45">
@@ -1005,304 +1019,313 @@
         <v>200</v>
       </c>
       <c r="F51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B53" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" t="s">
+        <v>39</v>
+      </c>
+      <c r="E53">
+        <v>404</v>
+      </c>
+      <c r="F53" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" t="s">
+        <v>53</v>
+      </c>
+      <c r="H53" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D54" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>403</v>
+      </c>
+      <c r="F54" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E55">
+        <v>403</v>
+      </c>
+      <c r="F55" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E56">
+        <v>200</v>
+      </c>
+      <c r="F56" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
         <v>28</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B58" t="s">
         <v>3</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C58" t="s">
         <v>12</v>
       </c>
-      <c r="G53" t="s">
+      <c r="E58">
+        <v>200</v>
+      </c>
+      <c r="G58" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B55" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B60" t="s">
         <v>10</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C60" t="s">
         <v>12</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D60" t="s">
         <v>39</v>
       </c>
-      <c r="E55">
+      <c r="E60">
         <v>413</v>
       </c>
-      <c r="F55" t="s">
-        <v>51</v>
-      </c>
-      <c r="H55" s="4" t="s">
+      <c r="F60" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D56" s="4" t="s">
+      <c r="H60" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D61" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E56">
+      <c r="E61">
         <v>404</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F61" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D57" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D62" t="s">
         <v>30</v>
       </c>
-      <c r="E57">
-        <v>403</v>
-      </c>
-      <c r="F57" t="s">
+      <c r="E62">
+        <v>403</v>
+      </c>
+      <c r="F62" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D58" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D63" t="s">
         <v>31</v>
       </c>
-      <c r="E58">
+      <c r="E63">
+        <v>403</v>
+      </c>
+      <c r="F63" t="s">
+        <v>37</v>
+      </c>
+      <c r="G63" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="D64" t="s">
+        <v>32</v>
+      </c>
+      <c r="E64">
+        <v>403</v>
+      </c>
+      <c r="F64" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D65" t="s">
+        <v>34</v>
+      </c>
+      <c r="E65">
         <v>201</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G65" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D59" t="s">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G66" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G67" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G68" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G69" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G70" t="s">
         <v>32</v>
       </c>
-      <c r="G59" t="s">
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G71" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B73" t="s">
+        <v>21</v>
+      </c>
+      <c r="C73" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" t="s">
+        <v>39</v>
+      </c>
+      <c r="E73" s="2">
+        <v>404</v>
+      </c>
+      <c r="F73" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D74" t="s">
+        <v>42</v>
+      </c>
+      <c r="E74">
+        <v>404</v>
+      </c>
+      <c r="F74" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D75" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D60" t="s">
+      <c r="E75">
+        <v>403</v>
+      </c>
+      <c r="F75" t="s">
+        <v>38</v>
+      </c>
+      <c r="H75" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D76" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E76">
+        <v>403</v>
+      </c>
+      <c r="F76" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D77" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E77">
+        <v>200</v>
+      </c>
+      <c r="G77" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D78" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D79" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D80" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G60" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G61" t="s">
+      <c r="G80" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G62" t="s">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G81" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G63" t="s">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G82" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G64" t="s">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G83" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B66" t="s">
-        <v>21</v>
-      </c>
-      <c r="C66" t="s">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B85" t="s">
+        <v>24</v>
+      </c>
+      <c r="C85" t="s">
         <v>12</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D85" t="s">
         <v>39</v>
       </c>
-      <c r="E66" s="2">
+      <c r="E85" s="2">
         <v>404</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F85" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D67" t="s">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D86" t="s">
         <v>42</v>
       </c>
-      <c r="E67">
+      <c r="E86">
         <v>404</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F86" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D68" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E68">
-        <v>403</v>
-      </c>
-      <c r="F68" t="s">
-        <v>38</v>
-      </c>
-      <c r="H68" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D69" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E69">
-        <v>403</v>
-      </c>
-      <c r="F69" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D70" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E70">
-        <v>200</v>
-      </c>
-      <c r="G70" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D71" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D72" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D73" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G74" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G75" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G76" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B78" t="s">
-        <v>24</v>
-      </c>
-      <c r="C78" t="s">
-        <v>12</v>
-      </c>
-      <c r="D78" t="s">
-        <v>39</v>
-      </c>
-      <c r="E78" s="2">
-        <v>404</v>
-      </c>
-      <c r="F78" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D79" t="s">
-        <v>42</v>
-      </c>
-      <c r="E79">
-        <v>404</v>
-      </c>
-      <c r="F79" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E80">
-        <v>403</v>
-      </c>
-      <c r="F80" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E81">
-        <v>403</v>
-      </c>
-      <c r="F81" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E82">
-        <v>200</v>
-      </c>
-      <c r="F82" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B84" t="s">
-        <v>24</v>
-      </c>
-      <c r="C84" t="s">
-        <v>23</v>
-      </c>
-      <c r="D84" t="s">
-        <v>39</v>
-      </c>
-      <c r="E84" s="2">
-        <v>404</v>
-      </c>
-      <c r="F84" t="s">
-        <v>35</v>
-      </c>
-      <c r="H84" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D85" t="s">
-        <v>42</v>
-      </c>
-      <c r="E85">
-        <v>404</v>
-      </c>
-      <c r="F85" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E86">
-        <v>403</v>
-      </c>
-      <c r="F86" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.45">
@@ -1310,63 +1333,138 @@
         <v>403</v>
       </c>
       <c r="F87" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.45">
       <c r="E88">
+        <v>403</v>
+      </c>
+      <c r="F88" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E89">
         <v>200</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F89" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B91" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C91" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D91" t="s">
-        <v>47</v>
-      </c>
-      <c r="E91">
-        <v>200</v>
+        <v>39</v>
+      </c>
+      <c r="E91" s="2">
+        <v>404</v>
+      </c>
+      <c r="F91" t="s">
+        <v>35</v>
+      </c>
+      <c r="H91" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D92" t="s">
+        <v>42</v>
+      </c>
+      <c r="E92">
+        <v>404</v>
+      </c>
+      <c r="F92" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E93">
+        <v>403</v>
+      </c>
+      <c r="F93" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E94">
+        <v>403</v>
+      </c>
+      <c r="F94" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E95">
+        <v>200</v>
+      </c>
+      <c r="F95" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B97" t="s">
+        <v>3</v>
+      </c>
+      <c r="C97" t="s">
+        <v>41</v>
+      </c>
+      <c r="D97" t="s">
+        <v>46</v>
+      </c>
+      <c r="E97">
+        <v>200</v>
+      </c>
+      <c r="G97" t="s">
+        <v>56</v>
+      </c>
+      <c r="K97" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D98" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D93" t="s">
+    <row r="99" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D99" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D94" t="s">
+    <row r="100" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D100" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D95" s="3" t="s">
+    <row r="101" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D101" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K101" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D102" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D96" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D97" t="s">
+      <c r="K102" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D103" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D98" t="s">
+    <row r="104" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D104" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added GET my Services (backend) added GET Services of User (backend)
</commit_message>
<xml_diff>
--- a/docs/Overwiew_endpoints.xlsx
+++ b/docs/Overwiew_endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\ese2019-team8\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="114_{370FD315-8FA4-4C58-8A8E-74881233F0BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3394C93D-52CB-43E7-8479-323B014CC8C5}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="114_{370FD315-8FA4-4C58-8A8E-74881233F0BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FF189DA1-ECC4-4557-83A4-F4C5DE9313F3}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="61">
   <si>
     <t>username</t>
   </si>
@@ -202,6 +202,18 @@
   </si>
   <si>
     <t>Array aller passender Services</t>
+  </si>
+  <si>
+    <t>Array aller eigenen Services</t>
+  </si>
+  <si>
+    <t>/myServices/:token</t>
+  </si>
+  <si>
+    <t>/servicesOf/:username</t>
+  </si>
+  <si>
+    <t>Array aller Services des Users</t>
   </si>
 </sst>
 </file>
@@ -575,9 +587,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B759F60C-B498-4DED-A37F-801BD6AC74F2}">
-  <dimension ref="A1:K104"/>
+  <dimension ref="A1:K111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1091,304 +1105,293 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B60" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>58</v>
+      </c>
+      <c r="E60" s="2">
+        <v>404</v>
+      </c>
+      <c r="F60" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E61">
+        <v>403</v>
+      </c>
+      <c r="F61" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E62">
+        <v>200</v>
+      </c>
+      <c r="G62" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B64" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" t="s">
+        <v>59</v>
+      </c>
+      <c r="E64" s="2">
+        <v>404</v>
+      </c>
+      <c r="F64" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E65">
+        <v>200</v>
+      </c>
+      <c r="G65" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B67" t="s">
         <v>10</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C67" t="s">
         <v>12</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D67" t="s">
         <v>39</v>
       </c>
-      <c r="E60">
+      <c r="E67">
         <v>413</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F67" t="s">
         <v>50</v>
       </c>
-      <c r="H60" s="4" t="s">
+      <c r="H67" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D61" s="4" t="s">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D68" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E61">
+      <c r="E68">
         <v>404</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F68" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D62" t="s">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D69" t="s">
         <v>30</v>
       </c>
-      <c r="E62">
-        <v>403</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="E69">
+        <v>403</v>
+      </c>
+      <c r="F69" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D63" t="s">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D70" t="s">
         <v>31</v>
       </c>
-      <c r="E63">
-        <v>403</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="E70">
+        <v>403</v>
+      </c>
+      <c r="F70" t="s">
         <v>37</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G70" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D64" t="s">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D71" t="s">
         <v>32</v>
       </c>
-      <c r="E64">
-        <v>403</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="E71">
+        <v>403</v>
+      </c>
+      <c r="F71" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D65" t="s">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D72" t="s">
         <v>34</v>
       </c>
-      <c r="E65">
+      <c r="E72">
         <v>201</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G72" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G66" t="s">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G73" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G67" t="s">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G74" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G68" t="s">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G75" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G69" t="s">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G76" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G70" t="s">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G77" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G71" t="s">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G78" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B73" t="s">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B80" t="s">
         <v>21</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C80" t="s">
         <v>12</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D80" t="s">
         <v>39</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E80" s="2">
         <v>404</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F80" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D74" t="s">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D81" t="s">
         <v>42</v>
       </c>
-      <c r="E74">
+      <c r="E81">
         <v>404</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F81" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D75" s="1" t="s">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D82" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E75">
-        <v>403</v>
-      </c>
-      <c r="F75" t="s">
+      <c r="E82">
+        <v>403</v>
+      </c>
+      <c r="F82" t="s">
         <v>38</v>
       </c>
-      <c r="H75" t="s">
+      <c r="H82" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D76" s="1" t="s">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D83" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E76">
-        <v>403</v>
-      </c>
-      <c r="F76" t="s">
+      <c r="E83">
+        <v>403</v>
+      </c>
+      <c r="F83" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D77" s="1" t="s">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D84" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E77">
+      <c r="E84">
         <v>200</v>
       </c>
-      <c r="G77" t="s">
+      <c r="G84" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D78" s="1" t="s">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D85" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G78" s="1" t="s">
+      <c r="G85" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D79" s="1" t="s">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D86" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G79" s="1" t="s">
+      <c r="G86" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D80" s="1" t="s">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D87" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G80" s="1" t="s">
+      <c r="G87" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G81" s="1" t="s">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G88" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G82" s="1" t="s">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G89" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G83" s="1" t="s">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G90" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B85" t="s">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B92" t="s">
         <v>24</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C92" t="s">
         <v>12</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D92" t="s">
         <v>39</v>
       </c>
-      <c r="E85" s="2">
+      <c r="E92" s="2">
         <v>404</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F92" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D86" t="s">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D93" t="s">
         <v>42</v>
       </c>
-      <c r="E86">
+      <c r="E93">
         <v>404</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F93" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E87">
-        <v>403</v>
-      </c>
-      <c r="F87" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E88">
-        <v>403</v>
-      </c>
-      <c r="F88" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E89">
-        <v>200</v>
-      </c>
-      <c r="F89" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B91" t="s">
-        <v>24</v>
-      </c>
-      <c r="C91" t="s">
-        <v>23</v>
-      </c>
-      <c r="D91" t="s">
-        <v>39</v>
-      </c>
-      <c r="E91" s="2">
-        <v>404</v>
-      </c>
-      <c r="F91" t="s">
-        <v>35</v>
-      </c>
-      <c r="H91" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D92" t="s">
-        <v>42</v>
-      </c>
-      <c r="E92">
-        <v>404</v>
-      </c>
-      <c r="F92" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E93">
-        <v>403</v>
-      </c>
-      <c r="F93" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.45">
@@ -1396,75 +1399,138 @@
         <v>403</v>
       </c>
       <c r="F94" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.45">
       <c r="E95">
+        <v>403</v>
+      </c>
+      <c r="F95" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E96">
         <v>200</v>
       </c>
-      <c r="F95" t="s">
+      <c r="F96" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B97" t="s">
-        <v>3</v>
-      </c>
-      <c r="C97" t="s">
-        <v>41</v>
-      </c>
-      <c r="D97" t="s">
-        <v>46</v>
-      </c>
-      <c r="E97">
-        <v>200</v>
-      </c>
-      <c r="G97" t="s">
-        <v>56</v>
-      </c>
-      <c r="K97" t="s">
-        <v>51</v>
-      </c>
-    </row>
     <row r="98" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B98" t="s">
+        <v>24</v>
+      </c>
+      <c r="C98" t="s">
+        <v>23</v>
+      </c>
       <c r="D98" t="s">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="E98" s="2">
+        <v>404</v>
+      </c>
+      <c r="F98" t="s">
+        <v>35</v>
+      </c>
+      <c r="H98" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="99" spans="2:11" x14ac:dyDescent="0.45">
       <c r="D99" t="s">
+        <v>42</v>
+      </c>
+      <c r="E99">
+        <v>404</v>
+      </c>
+      <c r="F99" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="E100">
+        <v>403</v>
+      </c>
+      <c r="F100" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="E101">
+        <v>403</v>
+      </c>
+      <c r="F101" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="E102">
+        <v>200</v>
+      </c>
+      <c r="F102" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="104" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B104" t="s">
+        <v>3</v>
+      </c>
+      <c r="C104" t="s">
+        <v>41</v>
+      </c>
+      <c r="D104" t="s">
+        <v>46</v>
+      </c>
+      <c r="E104">
+        <v>200</v>
+      </c>
+      <c r="G104" t="s">
+        <v>56</v>
+      </c>
+      <c r="K104" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D105" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D106" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="D100" t="s">
+    <row r="107" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D107" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="D101" s="3" t="s">
+    <row r="108" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D108" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K101" t="s">
+      <c r="K108" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="D102" s="3" t="s">
+    <row r="109" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D109" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="K102" t="s">
+      <c r="K109" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="D103" t="s">
+    <row r="110" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D110" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="D104" t="s">
+    <row r="111" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D111" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added searchAny function (backend)
</commit_message>
<xml_diff>
--- a/docs/Overwiew_endpoints.xlsx
+++ b/docs/Overwiew_endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\ese2019-team8\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="114_{370FD315-8FA4-4C58-8A8E-74881233F0BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FF189DA1-ECC4-4557-83A4-F4C5DE9313F3}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="114_{370FD315-8FA4-4C58-8A8E-74881233F0BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{42DD92D8-F788-41B4-9836-62DA2377DEF0}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="62">
   <si>
     <t>username</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>Array aller Services des Users</t>
+  </si>
+  <si>
+    <t>/searchAny/:searchString</t>
   </si>
 </sst>
 </file>
@@ -229,7 +232,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,12 +242,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -267,12 +264,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -587,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B759F60C-B498-4DED-A37F-801BD6AC74F2}">
-  <dimension ref="A1:K111"/>
+  <dimension ref="A1:K113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -702,7 +698,7 @@
       <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E11">
@@ -711,7 +707,7 @@
       <c r="F11" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -727,7 +723,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E13">
@@ -1171,12 +1167,12 @@
       <c r="F67" t="s">
         <v>50</v>
       </c>
-      <c r="H67" s="4" t="s">
+      <c r="H67" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E68">
@@ -1478,10 +1474,7 @@
         <v>3</v>
       </c>
       <c r="C104" t="s">
-        <v>41</v>
-      </c>
-      <c r="D104" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="E104">
         <v>200</v>
@@ -1493,44 +1486,58 @@
         <v>51</v>
       </c>
     </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="D105" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="106" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B106" t="s">
+        <v>3</v>
+      </c>
+      <c r="C106" t="s">
+        <v>41</v>
+      </c>
       <c r="D106" t="s">
-        <v>33</v>
+        <v>46</v>
+      </c>
+      <c r="E106">
+        <v>200</v>
+      </c>
+      <c r="G106" t="s">
+        <v>56</v>
+      </c>
+      <c r="K106" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="107" spans="2:11" x14ac:dyDescent="0.45">
       <c r="D107" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D108" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="109" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D109" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="108" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="D108" s="3" t="s">
+    <row r="110" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D110" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K108" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="D109" s="3" t="s">
+    </row>
+    <row r="111" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D111" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K109" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="D110" t="s">
+    </row>
+    <row r="112" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D112" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="111" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="D111" t="s">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D113" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added GET service by ID (backend)
</commit_message>
<xml_diff>
--- a/docs/Overwiew_endpoints.xlsx
+++ b/docs/Overwiew_endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\ese2019-team8\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="114_{370FD315-8FA4-4C58-8A8E-74881233F0BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{42DD92D8-F788-41B4-9836-62DA2377DEF0}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="114_{370FD315-8FA4-4C58-8A8E-74881233F0BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0B6CFB2D-A370-4E1C-ABFE-F829A8BD7F51}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{422A7462-8E4D-41BB-8F56-7537513871AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="64">
   <si>
     <t>username</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>/searchAny/:searchString</t>
+  </si>
+  <si>
+    <t>/id=:id</t>
+  </si>
+  <si>
+    <t>Service</t>
   </si>
 </sst>
 </file>
@@ -583,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B759F60C-B498-4DED-A37F-801BD6AC74F2}">
-  <dimension ref="A1:K113"/>
+  <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1104,43 +1110,43 @@
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E60" s="2">
         <v>404</v>
       </c>
       <c r="F60" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E61">
-        <v>403</v>
-      </c>
-      <c r="F61" t="s">
+        <v>200</v>
+      </c>
+      <c r="G61" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B63" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" t="s">
+        <v>58</v>
+      </c>
+      <c r="E63" s="2">
+        <v>404</v>
+      </c>
+      <c r="F63" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E64">
+        <v>403</v>
+      </c>
+      <c r="F64" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="E62">
-        <v>200</v>
-      </c>
-      <c r="G62" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B64" t="s">
-        <v>3</v>
-      </c>
-      <c r="C64" t="s">
-        <v>59</v>
-      </c>
-      <c r="E64" s="2">
-        <v>404</v>
-      </c>
-      <c r="F64" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.45">
@@ -1148,396 +1154,418 @@
         <v>200</v>
       </c>
       <c r="G65" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B67" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" t="s">
+        <v>59</v>
+      </c>
+      <c r="E67" s="2">
+        <v>404</v>
+      </c>
+      <c r="F67" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E68">
+        <v>200</v>
+      </c>
+      <c r="G68" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B70" t="s">
         <v>10</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C70" t="s">
         <v>12</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D70" t="s">
         <v>39</v>
       </c>
-      <c r="E67">
+      <c r="E70">
         <v>413</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F70" t="s">
         <v>50</v>
       </c>
-      <c r="H67" s="3" t="s">
+      <c r="H70" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D68" s="3" t="s">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D71" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E68">
-        <v>404</v>
-      </c>
-      <c r="F68" t="s">
+      <c r="E71">
+        <v>404</v>
+      </c>
+      <c r="F71" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D69" t="s">
-        <v>30</v>
-      </c>
-      <c r="E69">
-        <v>403</v>
-      </c>
-      <c r="F69" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D70" t="s">
-        <v>31</v>
-      </c>
-      <c r="E70">
-        <v>403</v>
-      </c>
-      <c r="F70" t="s">
-        <v>37</v>
-      </c>
-      <c r="G70" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D71" t="s">
-        <v>32</v>
-      </c>
-      <c r="E71">
-        <v>403</v>
-      </c>
-      <c r="F71" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D72" t="s">
+        <v>30</v>
+      </c>
+      <c r="E72">
+        <v>403</v>
+      </c>
+      <c r="F72" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D73" t="s">
+        <v>31</v>
+      </c>
+      <c r="E73">
+        <v>403</v>
+      </c>
+      <c r="F73" t="s">
+        <v>37</v>
+      </c>
+      <c r="G73" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D74" t="s">
+        <v>32</v>
+      </c>
+      <c r="E74">
+        <v>403</v>
+      </c>
+      <c r="F74" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D75" t="s">
         <v>34</v>
       </c>
-      <c r="E72">
+      <c r="E75">
         <v>201</v>
       </c>
-      <c r="G72" t="s">
+      <c r="G75" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G73" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G74" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G75" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G76" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G77" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.45">
       <c r="G78" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G79" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G80" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G81" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B80" t="s">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B83" t="s">
         <v>21</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C83" t="s">
         <v>12</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D83" t="s">
         <v>39</v>
       </c>
-      <c r="E80" s="2">
-        <v>404</v>
-      </c>
-      <c r="F80" t="s">
+      <c r="E83" s="2">
+        <v>404</v>
+      </c>
+      <c r="F83" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D81" t="s">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D84" t="s">
         <v>42</v>
       </c>
-      <c r="E81">
-        <v>404</v>
-      </c>
-      <c r="F81" t="s">
+      <c r="E84">
+        <v>404</v>
+      </c>
+      <c r="F84" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D82" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E82">
-        <v>403</v>
-      </c>
-      <c r="F82" t="s">
-        <v>38</v>
-      </c>
-      <c r="H82" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D83" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E83">
-        <v>403</v>
-      </c>
-      <c r="F83" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D84" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E84">
-        <v>200</v>
-      </c>
-      <c r="G84" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D85" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G85" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="E85">
+        <v>403</v>
+      </c>
+      <c r="F85" t="s">
+        <v>38</v>
+      </c>
+      <c r="H85" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D86" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G86" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="E86">
+        <v>403</v>
+      </c>
+      <c r="F86" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.45">
       <c r="D87" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E87">
+        <v>200</v>
+      </c>
+      <c r="G87" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D88" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D89" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D90" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G87" s="1" t="s">
+      <c r="G90" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G88" s="1" t="s">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G91" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G89" s="1" t="s">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G92" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G90" s="1" t="s">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="G93" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B92" t="s">
+    <row r="95" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B95" t="s">
         <v>24</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C95" t="s">
         <v>12</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D95" t="s">
         <v>39</v>
       </c>
-      <c r="E92" s="2">
-        <v>404</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="E95" s="2">
+        <v>404</v>
+      </c>
+      <c r="F95" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="D93" t="s">
+    <row r="96" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="D96" t="s">
         <v>42</v>
       </c>
-      <c r="E93">
-        <v>404</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="E96">
+        <v>404</v>
+      </c>
+      <c r="F96" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E94">
-        <v>403</v>
-      </c>
-      <c r="F94" t="s">
+    <row r="97" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="E97">
+        <v>403</v>
+      </c>
+      <c r="F97" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E95">
-        <v>403</v>
-      </c>
-      <c r="F95" t="s">
+    <row r="98" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="E98">
+        <v>403</v>
+      </c>
+      <c r="F98" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="E96">
-        <v>200</v>
-      </c>
-      <c r="F96" t="s">
+    <row r="99" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="E99">
+        <v>200</v>
+      </c>
+      <c r="F99" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B98" t="s">
+    <row r="101" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B101" t="s">
         <v>24</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C101" t="s">
         <v>23</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D101" t="s">
         <v>39</v>
       </c>
-      <c r="E98" s="2">
-        <v>404</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="E101" s="2">
+        <v>404</v>
+      </c>
+      <c r="F101" t="s">
         <v>35</v>
       </c>
-      <c r="H98" t="s">
+      <c r="H101" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="D99" t="s">
+    <row r="102" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D102" t="s">
         <v>42</v>
       </c>
-      <c r="E99">
-        <v>404</v>
-      </c>
-      <c r="F99" t="s">
+      <c r="E102">
+        <v>404</v>
+      </c>
+      <c r="F102" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="E100">
-        <v>403</v>
-      </c>
-      <c r="F100" t="s">
+    <row r="103" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="E103">
+        <v>403</v>
+      </c>
+      <c r="F103" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="E101">
-        <v>403</v>
-      </c>
-      <c r="F101" t="s">
+    <row r="104" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="E104">
+        <v>403</v>
+      </c>
+      <c r="F104" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="E102">
-        <v>200</v>
-      </c>
-      <c r="F102" t="s">
+    <row r="105" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="E105">
+        <v>200</v>
+      </c>
+      <c r="F105" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B104" t="s">
+    <row r="107" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B107" t="s">
         <v>3</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C107" t="s">
         <v>61</v>
       </c>
-      <c r="E104">
-        <v>200</v>
-      </c>
-      <c r="G104" t="s">
+      <c r="E107">
+        <v>200</v>
+      </c>
+      <c r="G107" t="s">
         <v>56</v>
       </c>
-      <c r="K104" t="s">
+      <c r="K107" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B106" t="s">
+    <row r="109" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B109" t="s">
         <v>3</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C109" t="s">
         <v>41</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D109" t="s">
         <v>46</v>
       </c>
-      <c r="E106">
-        <v>200</v>
-      </c>
-      <c r="G106" t="s">
+      <c r="E109">
+        <v>200</v>
+      </c>
+      <c r="G109" t="s">
         <v>56</v>
       </c>
-      <c r="K106" t="s">
+      <c r="K109" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="107" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="D107" t="s">
+    <row r="110" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D110" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="D108" t="s">
+    <row r="111" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="D111" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="D109" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="D110" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="111" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="D111" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="112" spans="2:11" x14ac:dyDescent="0.45">
       <c r="D112" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D113" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D114" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D115" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D113" t="s">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D116" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>